<commit_message>
added table generating code
</commit_message>
<xml_diff>
--- a/primary.xlsx
+++ b/primary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://egms-my.sharepoint.com/personal/gubh001_egms_no/Documents/guru_shared/Engineering-AI-enabled-software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2183" documentId="11_123976AF87B05CA1344901D04B5ED87656C97722" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B86E794-D837-4C27-8ABA-A8D547B2D8AF}"/>
+  <xr:revisionPtr revIDLastSave="2194" documentId="11_123976AF87B05CA1344901D04B5ED87656C97722" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98294019-5CA1-4E30-A91B-8937F0D6F21C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 20230328" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4011" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4010" uniqueCount="1249">
   <si>
     <t>Key</t>
   </si>
@@ -1133,26 +1133,28 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">All lifecycle phases addressed: </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>requirements, design, development, testing, operation</t>
+      <t xml:space="preserve">requirements, design, development, testing, operation
+</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 Table 2 provides long list of AI projects AND how SE methods were applied</t>
@@ -1329,26 +1331,27 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">Development </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>methodology</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>/</t>
     </r>
@@ -1356,20 +1359,16 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Design</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for AI-powered systems.
 How a methodology automates the AI development process if neural networks are changed or added to the system?</t>
@@ -1872,20 +1871,16 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>Design</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">- Concept based SE combining the objectives of component-based SE (productivity, extensibility, etc.) and ML (reinforcement learning- accuracy) </t>
     </r>
@@ -2478,7 +2473,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Human-centered design practices are realised in the context of developing AI applications.
 HCAI design constraints- developing AI applications that are trustworthy, usable, and based on human needs
@@ -2492,7 +2486,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">human </t>
     </r>
@@ -2501,7 +2494,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>and technology can solve problems in unforeseen ways as they work together (AI as an intelligent tool for a human)</t>
     </r>
@@ -2536,26 +2528,27 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">Design- Human-centered AI </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>design</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> in reality
 It's great to see many AI app domains presented :)
@@ -3581,16 +3574,19 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">All lifecycle phases addressed: </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">requirements, design, development, testing, operation
 </t>
@@ -3598,10 +3594,8 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 This paper is very similar to our study.</t>
@@ -4888,27 +4882,8 @@
     <t>will include the revision of the semantic model in order to reduce reasoning times for CPM’s software functionality retrieval</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Focuses more on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>design</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">Focuses more on design
 Its's hardware related - and software engineering is mentioned as mainstream </t>
-    </r>
   </si>
   <si>
     <t>borderline paper not directly related to ML</t>
@@ -5264,6 +5239,40 @@
   </si>
   <si>
     <t>deto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Human-centered design practices are realised in the context of developing AI applications.
+HCAI design constraints- developing AI applications that are trustworthy, usable, and based on human needs
+Human-centered AI principles:
+Explainable AI, Transparency, Ethical AI,  Fair AI, Trustworthy AI, Responsible AI, and Sustainable AI
+AI’s and HCI.. Studies investigating human-AI interaction highlights the potential this new kind of collaboration has – together the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">human </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>and technology can solve problems in unforeseen ways as they work together (AI as an intelligent tool for a human)</t>
+    </r>
   </si>
   <si>
     <t>It's great to see many AI app domains presented :)
@@ -5318,6 +5327,45 @@
   </si>
   <si>
     <t>Lwakatare2020</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Systems that rely on Machine Learning have differing demands on quality—known as non-functional requirements (NFRs)—from traditional systems.
+Focus on how NFRs are defined and measured over different aspects of a ML system (i.e., model, data, or whole system).
+Traditional NFRs like accuracy can still be important for ML, as new NFRs such as transparency, fairness, and explainability are gaining more importance. However, the level of importance of NFRs for ML systems varied based on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">background </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">of the participants; therefore, more research is needed in this area.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Most practitioners think of NFRs over the whole system, or over the model, few consider data.</t>
+    </r>
   </si>
   <si>
     <t>Testing for ML is different than testing of classic software systems. Therefore, you need different acceptance requirements.
@@ -5448,6 +5496,12 @@
     <t>This paper is focused on medical application of AI enabled software</t>
   </si>
   <si>
+    <t>software requirements: 
+• A lot of focus on NFRs for AI (10 of 17 studies), especially new AI-specific quality attributes
+• Several specification and notation approaches to deal with probabilistic results or ambiguity, e.g., partial specification 
+• Very few holistic views on the RE process for AI (only one study), focus on support for RE specification and derivation</t>
+  </si>
+  <si>
     <t>This paper is very similar to our study.</t>
   </si>
   <si>
@@ -6463,6 +6517,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t xml:space="preserve">Proposed a </t>
     </r>
     <r>
@@ -6471,8 +6530,6 @@
         <sz val="14"/>
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>continous development process</t>
     </r>
@@ -6481,8 +6538,6 @@
         <sz val="14"/>
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for machine-learning applications used in safety-critical applications: operational domain specification, data orchestration and preparation, model training (</t>
     </r>
@@ -6492,8 +6547,6 @@
         <sz val="14"/>
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>most researched</t>
     </r>
@@ -6502,8 +6555,6 @@
         <sz val="14"/>
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>) and model integration.</t>
     </r>
@@ -6710,7 +6761,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6926,6 +6977,17 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -7165,7 +7227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7454,6 +7516,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -7481,7 +7549,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7789,9 +7857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CBC91E-CDF2-4B90-A41B-09A813B27C4C}">
   <dimension ref="A1:EG43"/>
   <sheetViews>
-    <sheetView topLeftCell="DY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL4" sqref="AL4"/>
+    <sheetView tabSelected="1" topLeftCell="DY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="DW7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="EE8" sqref="EE8"/>
       <selection activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
@@ -8134,80 +8202,80 @@
       <c r="CN1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="106" t="s">
+      <c r="CO1" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="106"/>
-      <c r="CQ1" s="106"/>
-      <c r="CR1" s="106" t="s">
+      <c r="CP1" s="108"/>
+      <c r="CQ1" s="108"/>
+      <c r="CR1" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="CS1" s="106"/>
-      <c r="CT1" s="106"/>
-      <c r="CU1" s="104" t="s">
+      <c r="CS1" s="108"/>
+      <c r="CT1" s="108"/>
+      <c r="CU1" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="CV1" s="104"/>
-      <c r="CW1" s="104"/>
-      <c r="CX1" s="104" t="s">
+      <c r="CV1" s="106"/>
+      <c r="CW1" s="106"/>
+      <c r="CX1" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="CY1" s="104"/>
-      <c r="CZ1" s="104"/>
-      <c r="DA1" s="104" t="s">
+      <c r="CY1" s="106"/>
+      <c r="CZ1" s="106"/>
+      <c r="DA1" s="106" t="s">
         <v>95</v>
       </c>
-      <c r="DB1" s="104"/>
-      <c r="DC1" s="104"/>
-      <c r="DD1" s="104" t="s">
+      <c r="DB1" s="106"/>
+      <c r="DC1" s="106"/>
+      <c r="DD1" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="DE1" s="104"/>
-      <c r="DF1" s="104"/>
-      <c r="DG1" s="104" t="s">
+      <c r="DE1" s="106"/>
+      <c r="DF1" s="106"/>
+      <c r="DG1" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="DH1" s="104"/>
-      <c r="DI1" s="104"/>
-      <c r="DJ1" s="104" t="s">
+      <c r="DH1" s="106"/>
+      <c r="DI1" s="106"/>
+      <c r="DJ1" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="DK1" s="104"/>
-      <c r="DL1" s="104"/>
-      <c r="DM1" s="104" t="s">
+      <c r="DK1" s="106"/>
+      <c r="DL1" s="106"/>
+      <c r="DM1" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="DN1" s="104"/>
-      <c r="DO1" s="104"/>
-      <c r="DP1" s="104" t="s">
+      <c r="DN1" s="106"/>
+      <c r="DO1" s="106"/>
+      <c r="DP1" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="DQ1" s="104"/>
-      <c r="DR1" s="104"/>
-      <c r="DS1" s="104" t="s">
+      <c r="DQ1" s="106"/>
+      <c r="DR1" s="106"/>
+      <c r="DS1" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="DT1" s="104"/>
-      <c r="DU1" s="104"/>
-      <c r="DV1" s="104" t="s">
+      <c r="DT1" s="106"/>
+      <c r="DU1" s="106"/>
+      <c r="DV1" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="DW1" s="104"/>
-      <c r="DX1" s="104"/>
-      <c r="DY1" s="104" t="s">
+      <c r="DW1" s="106"/>
+      <c r="DX1" s="106"/>
+      <c r="DY1" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="DZ1" s="104"/>
-      <c r="EA1" s="104"/>
-      <c r="EB1" s="104" t="s">
+      <c r="DZ1" s="106"/>
+      <c r="EA1" s="106"/>
+      <c r="EB1" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="EC1" s="104"/>
-      <c r="ED1" s="104"/>
-      <c r="EE1" s="105" t="s">
+      <c r="EC1" s="106"/>
+      <c r="ED1" s="106"/>
+      <c r="EE1" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="EF1" s="105"/>
+      <c r="EF1" s="107"/>
       <c r="EG1" s="12"/>
     </row>
     <row r="2" spans="1:137" ht="56.25">
@@ -9738,7 +9806,7 @@
       </c>
       <c r="EG7" s="12"/>
     </row>
-    <row r="8" spans="1:137" ht="187.5">
+    <row r="8" spans="1:137" ht="189">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -9963,7 +10031,7 @@
         <v>316</v>
       </c>
       <c r="ED8" s="7"/>
-      <c r="EE8" s="7" t="s">
+      <c r="EE8" s="42" t="s">
         <v>317</v>
       </c>
       <c r="EF8" s="31" t="s">
@@ -10202,7 +10270,7 @@
       <c r="EF9" s="31"/>
       <c r="EG9" s="12"/>
     </row>
-    <row r="10" spans="1:137" ht="281.25">
+    <row r="10" spans="1:137" ht="283.5">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -10429,7 +10497,7 @@
         <v>181</v>
       </c>
       <c r="ED10" s="7"/>
-      <c r="EE10" s="7" t="s">
+      <c r="EE10" s="42" t="s">
         <v>364</v>
       </c>
       <c r="EF10" s="31"/>
@@ -11162,7 +11230,7 @@
       </c>
       <c r="EG13" s="12"/>
     </row>
-    <row r="14" spans="1:137" ht="337.5">
+    <row r="14" spans="1:137" ht="339.75">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -11401,7 +11469,7 @@
         <v>491</v>
       </c>
       <c r="ED14" s="7"/>
-      <c r="EE14" s="7" t="s">
+      <c r="EE14" s="42" t="s">
         <v>492</v>
       </c>
       <c r="EF14" s="30" t="s">
@@ -12369,7 +12437,7 @@
       </c>
       <c r="EG18" s="12"/>
     </row>
-    <row r="19" spans="1:137" ht="356.25">
+    <row r="19" spans="1:137" ht="339.75">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -12551,7 +12619,7 @@
         <v>181</v>
       </c>
       <c r="DI19" s="7"/>
-      <c r="DJ19" s="29" t="s">
+      <c r="DJ19" s="42" t="s">
         <v>612</v>
       </c>
       <c r="DK19" s="7" t="s">
@@ -12600,7 +12668,7 @@
         <v>620</v>
       </c>
       <c r="ED19" s="7"/>
-      <c r="EE19" s="7" t="s">
+      <c r="EE19" s="42" t="s">
         <v>621</v>
       </c>
       <c r="EF19" s="7" t="s">
@@ -12608,7 +12676,7 @@
       </c>
       <c r="EG19" s="12"/>
     </row>
-    <row r="20" spans="1:137" ht="356.25">
+    <row r="20" spans="1:137" ht="359.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -14010,7 +14078,7 @@
       </c>
       <c r="EG25" s="12"/>
     </row>
-    <row r="26" spans="1:137" ht="281.25">
+    <row r="26" spans="1:137" ht="283.5">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -14243,7 +14311,7 @@
         <v>785</v>
       </c>
       <c r="ED26" s="5"/>
-      <c r="EE26" s="5" t="s">
+      <c r="EE26" s="115" t="s">
         <v>786</v>
       </c>
       <c r="EF26" s="34" t="s">
@@ -14251,7 +14319,7 @@
       </c>
       <c r="EG26" s="12"/>
     </row>
-    <row r="27" spans="1:137" ht="375">
+    <row r="27" spans="1:137" ht="378">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -15452,7 +15520,7 @@
       </c>
       <c r="EG31" s="12"/>
     </row>
-    <row r="32" spans="1:137" ht="375">
+    <row r="32" spans="1:137" ht="378">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -15693,7 +15761,7 @@
       </c>
       <c r="EG32" s="12"/>
     </row>
-    <row r="33" spans="1:137" ht="409.5">
+    <row r="33" spans="1:137" ht="409.6">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -16993,7 +17061,7 @@
       </c>
       <c r="EG38" s="12"/>
     </row>
-    <row r="39" spans="1:137" ht="216">
+    <row r="39" spans="1:137" ht="248.25">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -17982,8 +18050,8 @@
   <dimension ref="A1:EG52"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="EB2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="EB30" sqref="EB30"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -18325,80 +18393,80 @@
       <c r="CN1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="106" t="s">
+      <c r="CO1" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="106"/>
-      <c r="CQ1" s="106"/>
-      <c r="CR1" s="106" t="s">
+      <c r="CP1" s="108"/>
+      <c r="CQ1" s="108"/>
+      <c r="CR1" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="CS1" s="106"/>
-      <c r="CT1" s="106"/>
-      <c r="CU1" s="104" t="s">
+      <c r="CS1" s="108"/>
+      <c r="CT1" s="108"/>
+      <c r="CU1" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="CV1" s="104"/>
-      <c r="CW1" s="104"/>
-      <c r="CX1" s="104" t="s">
+      <c r="CV1" s="106"/>
+      <c r="CW1" s="106"/>
+      <c r="CX1" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="CY1" s="104"/>
-      <c r="CZ1" s="104"/>
-      <c r="DA1" s="104" t="s">
+      <c r="CY1" s="106"/>
+      <c r="CZ1" s="106"/>
+      <c r="DA1" s="106" t="s">
         <v>95</v>
       </c>
-      <c r="DB1" s="104"/>
-      <c r="DC1" s="104"/>
-      <c r="DD1" s="104" t="s">
+      <c r="DB1" s="106"/>
+      <c r="DC1" s="106"/>
+      <c r="DD1" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="DE1" s="104"/>
-      <c r="DF1" s="104"/>
-      <c r="DG1" s="104" t="s">
+      <c r="DE1" s="106"/>
+      <c r="DF1" s="106"/>
+      <c r="DG1" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="DH1" s="104"/>
-      <c r="DI1" s="104"/>
-      <c r="DJ1" s="104" t="s">
+      <c r="DH1" s="106"/>
+      <c r="DI1" s="106"/>
+      <c r="DJ1" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="DK1" s="104"/>
-      <c r="DL1" s="104"/>
-      <c r="DM1" s="104" t="s">
+      <c r="DK1" s="106"/>
+      <c r="DL1" s="106"/>
+      <c r="DM1" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="DN1" s="104"/>
-      <c r="DO1" s="104"/>
-      <c r="DP1" s="104" t="s">
+      <c r="DN1" s="106"/>
+      <c r="DO1" s="106"/>
+      <c r="DP1" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="DQ1" s="104"/>
-      <c r="DR1" s="104"/>
-      <c r="DS1" s="104" t="s">
+      <c r="DQ1" s="106"/>
+      <c r="DR1" s="106"/>
+      <c r="DS1" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="DT1" s="104"/>
-      <c r="DU1" s="104"/>
-      <c r="DV1" s="104" t="s">
+      <c r="DT1" s="106"/>
+      <c r="DU1" s="106"/>
+      <c r="DV1" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="DW1" s="104"/>
-      <c r="DX1" s="104"/>
-      <c r="DY1" s="104" t="s">
+      <c r="DW1" s="106"/>
+      <c r="DX1" s="106"/>
+      <c r="DY1" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="DZ1" s="104"/>
-      <c r="EA1" s="104"/>
-      <c r="EB1" s="104" t="s">
+      <c r="DZ1" s="106"/>
+      <c r="EA1" s="106"/>
+      <c r="EB1" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="EC1" s="104"/>
-      <c r="ED1" s="104"/>
-      <c r="EE1" s="105" t="s">
+      <c r="EC1" s="106"/>
+      <c r="ED1" s="106"/>
+      <c r="EE1" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="EF1" s="105"/>
+      <c r="EF1" s="107"/>
       <c r="EG1" s="12"/>
     </row>
     <row r="2" spans="1:137" ht="56.25">
@@ -19470,7 +19538,7 @@
       <c r="EF5" s="31"/>
       <c r="EG5" s="12"/>
     </row>
-    <row r="6" spans="1:137" ht="262.5">
+    <row r="6" spans="1:137" ht="264.75">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -20161,7 +20229,7 @@
       </c>
       <c r="EG8" s="12"/>
     </row>
-    <row r="9" spans="1:137" ht="187.5">
+    <row r="9" spans="1:137" ht="189">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -23306,7 +23374,7 @@
       </c>
       <c r="DI22" s="7"/>
       <c r="DJ22" s="29" t="s">
-        <v>612</v>
+        <v>1131</v>
       </c>
       <c r="DK22" s="7" t="s">
         <v>613</v>
@@ -23355,7 +23423,7 @@
       </c>
       <c r="ED22" s="7"/>
       <c r="EE22" s="7" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="EF22" s="31" t="s">
         <v>622</v>
@@ -23367,7 +23435,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>529</v>
@@ -23391,10 +23459,10 @@
         <v>274</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="N23" s="19">
         <v>2021</v>
@@ -23407,7 +23475,7 @@
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="17" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="S23" s="17"/>
       <c r="T23" s="17"/>
@@ -23416,7 +23484,7 @@
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
       <c r="Y23" s="17" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="Z23" s="17"/>
       <c r="AA23" s="17"/>
@@ -23431,7 +23499,7 @@
       <c r="AJ23" s="17"/>
       <c r="AK23" s="17"/>
       <c r="AL23" s="17" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="AM23" s="17"/>
       <c r="AN23" s="17" t="s">
@@ -23513,7 +23581,7 @@
       </c>
       <c r="CU23" s="18"/>
       <c r="CV23" s="18" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="CW23" s="18"/>
       <c r="CX23" s="18"/>
@@ -23785,7 +23853,7 @@
       </c>
       <c r="ED24" s="7"/>
       <c r="EE24" s="7" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="EF24" s="31" t="s">
         <v>648</v>
@@ -23797,7 +23865,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>529</v>
@@ -23812,7 +23880,7 @@
         <v>320</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -23821,10 +23889,10 @@
         <v>323</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="N25" s="19">
         <v>2020</v>
@@ -23844,7 +23912,7 @@
       <c r="W25" s="17"/>
       <c r="X25" s="17"/>
       <c r="Y25" s="17" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="Z25" s="17"/>
       <c r="AA25" s="17"/>
@@ -23859,7 +23927,7 @@
       <c r="AJ25" s="17"/>
       <c r="AK25" s="17"/>
       <c r="AL25" s="17" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="AM25" s="17"/>
       <c r="AN25" s="17" t="s">
@@ -23941,7 +24009,7 @@
       </c>
       <c r="CU25" s="18"/>
       <c r="CV25" s="18" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="CW25" s="18"/>
       <c r="CX25" s="18"/>
@@ -23981,7 +24049,7 @@
       <c r="EF25" s="32"/>
       <c r="EG25" s="20"/>
     </row>
-    <row r="26" spans="1:137" ht="393.75">
+    <row r="26" spans="1:137" ht="396.75">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -24152,8 +24220,8 @@
       </c>
       <c r="DE26" s="7"/>
       <c r="DF26" s="7"/>
-      <c r="DG26" s="29" t="s">
-        <v>660</v>
+      <c r="DG26" s="42" t="s">
+        <v>1147</v>
       </c>
       <c r="DH26" s="7"/>
       <c r="DI26" s="7"/>
@@ -24168,7 +24236,7 @@
       <c r="DN26" s="7"/>
       <c r="DO26" s="7"/>
       <c r="DP26" s="7" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="DQ26" s="7"/>
       <c r="DR26" s="7"/>
@@ -24371,7 +24439,7 @@
       </c>
       <c r="DC27" s="7"/>
       <c r="DD27" s="7" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="DE27" s="7" t="s">
         <v>680</v>
@@ -24402,7 +24470,7 @@
         <v>686</v>
       </c>
       <c r="DQ27" s="7" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="DR27" s="7"/>
       <c r="DS27" s="7" t="s">
@@ -24675,7 +24743,7 @@
       </c>
       <c r="ED28" s="7"/>
       <c r="EE28" s="7" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="EF28" s="73" t="s">
         <v>718</v>
@@ -24896,7 +24964,7 @@
       <c r="EC29" s="71"/>
       <c r="ED29" s="71"/>
       <c r="EE29" s="71" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="EF29" s="47"/>
       <c r="EG29" s="12"/>
@@ -25074,7 +25142,7 @@
       </c>
       <c r="DC30" s="7"/>
       <c r="DD30" s="29" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="DE30" s="7" t="s">
         <v>743</v>
@@ -25100,7 +25168,7 @@
       <c r="DN30" s="7"/>
       <c r="DO30" s="7"/>
       <c r="DP30" s="29" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="DQ30" s="7" t="s">
         <v>749</v>
@@ -25135,14 +25203,14 @@
       </c>
       <c r="ED30" s="7"/>
       <c r="EE30" s="7" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="EF30" s="31" t="s">
         <v>758</v>
       </c>
       <c r="EG30" s="12"/>
     </row>
-    <row r="31" spans="1:137" ht="281.25">
+    <row r="31" spans="1:137" ht="283.5">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -25323,7 +25391,7 @@
       <c r="DF31" s="5"/>
       <c r="DG31" s="5"/>
       <c r="DH31" s="5" t="s">
-        <v>773</v>
+        <v>1156</v>
       </c>
       <c r="DI31" s="5"/>
       <c r="DJ31" s="5" t="s">
@@ -25376,7 +25444,7 @@
       </c>
       <c r="ED31" s="5"/>
       <c r="EE31" s="5" t="s">
-        <v>1154</v>
+        <v>1157</v>
       </c>
       <c r="EF31" s="34" t="s">
         <v>787</v>
@@ -25388,7 +25456,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>1155</v>
+        <v>1158</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>529</v>
@@ -25412,10 +25480,10 @@
         <v>223</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>1156</v>
+        <v>1159</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>1157</v>
+        <v>1160</v>
       </c>
       <c r="N32" s="19">
         <v>2021</v>
@@ -25428,7 +25496,7 @@
       </c>
       <c r="Q32" s="19"/>
       <c r="R32" s="17" t="s">
-        <v>1158</v>
+        <v>1161</v>
       </c>
       <c r="S32" s="17"/>
       <c r="T32" s="17"/>
@@ -25452,7 +25520,7 @@
       <c r="AJ32" s="17"/>
       <c r="AK32" s="17"/>
       <c r="AL32" s="17" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
       <c r="AM32" s="17"/>
       <c r="AN32" s="17" t="s">
@@ -25534,7 +25602,7 @@
       </c>
       <c r="CU32" s="18"/>
       <c r="CV32" s="18" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="CW32" s="18"/>
       <c r="CX32" s="18"/>
@@ -25816,7 +25884,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>529</v>
@@ -25840,10 +25908,10 @@
         <v>428</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
       <c r="N34" s="19">
         <v>2019</v>
@@ -25856,7 +25924,7 @@
       </c>
       <c r="Q34" s="19"/>
       <c r="R34" s="17" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
@@ -25865,7 +25933,7 @@
       <c r="W34" s="17"/>
       <c r="X34" s="17"/>
       <c r="Y34" s="17" t="s">
-        <v>1164</v>
+        <v>1167</v>
       </c>
       <c r="Z34" s="17"/>
       <c r="AA34" s="17"/>
@@ -25880,7 +25948,7 @@
       <c r="AJ34" s="17"/>
       <c r="AK34" s="17"/>
       <c r="AL34" s="17" t="s">
-        <v>1165</v>
+        <v>1168</v>
       </c>
       <c r="AM34" s="17"/>
       <c r="AN34" s="17" t="s">
@@ -25962,7 +26030,7 @@
       </c>
       <c r="CU34" s="18"/>
       <c r="CV34" s="18" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="CW34" s="18"/>
       <c r="CX34" s="18"/>
@@ -26002,7 +26070,7 @@
       <c r="EF34" s="32"/>
       <c r="EG34" s="20"/>
     </row>
-    <row r="35" spans="1:137" ht="375">
+    <row r="35" spans="1:137" ht="378">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -26236,7 +26304,7 @@
       </c>
       <c r="ED35" s="7"/>
       <c r="EE35" s="42" t="s">
-        <v>1166</v>
+        <v>1169</v>
       </c>
       <c r="EF35" s="31" t="s">
         <v>826</v>
@@ -26477,7 +26545,7 @@
       </c>
       <c r="ED36" s="7"/>
       <c r="EE36" s="7" t="s">
-        <v>1167</v>
+        <v>1170</v>
       </c>
       <c r="EF36" s="31" t="s">
         <v>850</v>
@@ -26718,7 +26786,7 @@
       </c>
       <c r="ED37" s="7"/>
       <c r="EE37" s="42" t="s">
-        <v>1168</v>
+        <v>1171</v>
       </c>
       <c r="EF37" s="31" t="s">
         <v>866</v>
@@ -26730,7 +26798,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>1169</v>
+        <v>1172</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>529</v>
@@ -26745,7 +26813,7 @@
         <v>366</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>1170</v>
+        <v>1173</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>368</v>
@@ -26756,10 +26824,10 @@
         <v>370</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>1171</v>
+        <v>1174</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>1172</v>
+        <v>1175</v>
       </c>
       <c r="N38" s="19">
         <v>2022</v>
@@ -26772,7 +26840,7 @@
       </c>
       <c r="Q38" s="19"/>
       <c r="R38" s="17" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="S38" s="17"/>
       <c r="T38" s="17">
@@ -26798,7 +26866,7 @@
       <c r="AJ38" s="17"/>
       <c r="AK38" s="17"/>
       <c r="AL38" s="17" t="s">
-        <v>1174</v>
+        <v>1177</v>
       </c>
       <c r="AM38" s="17"/>
       <c r="AN38" s="17" t="s">
@@ -26880,7 +26948,7 @@
       </c>
       <c r="CU38" s="18"/>
       <c r="CV38" s="18" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="CW38" s="18"/>
       <c r="CX38" s="18"/>
@@ -27084,7 +27152,7 @@
       </c>
       <c r="CZ39" s="7"/>
       <c r="DA39" s="7" t="s">
-        <v>1175</v>
+        <v>1178</v>
       </c>
       <c r="DB39" s="7" t="s">
         <v>879</v>
@@ -27154,14 +27222,14 @@
       </c>
       <c r="ED39" s="7"/>
       <c r="EE39" s="7" t="s">
-        <v>1176</v>
+        <v>1179</v>
       </c>
       <c r="EF39" s="31" t="s">
         <v>885</v>
       </c>
       <c r="EG39" s="12"/>
     </row>
-    <row r="40" spans="1:137" ht="375">
+    <row r="40" spans="1:137" ht="378">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -27395,14 +27463,14 @@
       </c>
       <c r="ED40" s="7"/>
       <c r="EE40" s="7" t="s">
-        <v>1177</v>
+        <v>1180</v>
       </c>
       <c r="EF40" s="31" t="s">
         <v>912</v>
       </c>
       <c r="EG40" s="12"/>
     </row>
-    <row r="41" spans="1:137" ht="409.5">
+    <row r="41" spans="1:137" ht="409.6">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -27611,7 +27679,7 @@
         <v>935</v>
       </c>
       <c r="DT41" s="7" t="s">
-        <v>1178</v>
+        <v>1181</v>
       </c>
       <c r="DU41" s="7"/>
       <c r="DV41" s="7" t="s">
@@ -27636,7 +27704,7 @@
       </c>
       <c r="ED41" s="7"/>
       <c r="EE41" s="7" t="s">
-        <v>1179</v>
+        <v>1182</v>
       </c>
       <c r="EF41" s="31" t="s">
         <v>941</v>
@@ -28076,7 +28144,7 @@
       </c>
       <c r="ED43" s="7"/>
       <c r="EE43" s="7" t="s">
-        <v>1180</v>
+        <v>1183</v>
       </c>
       <c r="EF43" s="73" t="s">
         <v>982</v>
@@ -28279,7 +28347,7 @@
       </c>
       <c r="ED44" s="55"/>
       <c r="EE44" s="55" t="s">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="EF44" s="47" t="s">
         <v>997</v>
@@ -28482,7 +28550,7 @@
       </c>
       <c r="ED45" s="55"/>
       <c r="EE45" s="55" t="s">
-        <v>1182</v>
+        <v>1185</v>
       </c>
       <c r="EF45" s="47" t="s">
         <v>1015</v>
@@ -28888,7 +28956,7 @@
       </c>
       <c r="ED47" s="55"/>
       <c r="EE47" s="55" t="s">
-        <v>1183</v>
+        <v>1186</v>
       </c>
       <c r="EF47" s="47" t="s">
         <v>1041</v>
@@ -29091,14 +29159,14 @@
       </c>
       <c r="ED48" s="55"/>
       <c r="EE48" s="55" t="s">
-        <v>1184</v>
+        <v>1187</v>
       </c>
       <c r="EF48" s="47" t="s">
         <v>1059</v>
       </c>
       <c r="EG48" s="12"/>
     </row>
-    <row r="49" spans="1:137" ht="396">
+    <row r="49" spans="1:137" ht="372">
       <c r="A49" s="37">
         <v>47</v>
       </c>
@@ -29237,9 +29305,7 @@
         <v>1068</v>
       </c>
       <c r="DF49" s="55"/>
-      <c r="DG49" s="55" t="s">
-        <v>1069</v>
-      </c>
+      <c r="DG49" s="55"/>
       <c r="DH49" s="55" t="s">
         <v>181</v>
       </c>
@@ -29294,7 +29360,7 @@
       </c>
       <c r="ED49" s="55"/>
       <c r="EE49" s="55" t="s">
-        <v>1185</v>
+        <v>1188</v>
       </c>
       <c r="EF49" s="47" t="s">
         <v>1074</v>
@@ -29509,18 +29575,18 @@
         <v>49</v>
       </c>
       <c r="B51" s="61" t="s">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="C51" s="62"/>
       <c r="D51" s="63" t="s">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="E51" s="64">
         <v>2021</v>
       </c>
       <c r="F51" s="65"/>
       <c r="G51" s="66" t="s">
-        <v>1188</v>
+        <v>1191</v>
       </c>
       <c r="H51" s="67"/>
       <c r="I51" s="65"/>
@@ -29654,7 +29720,7 @@
       <c r="EC51" s="67"/>
       <c r="ED51" s="67"/>
       <c r="EE51" s="67" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
       <c r="EF51" s="44"/>
       <c r="EG51" s="45"/>
@@ -29827,8 +29893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6F72FB-478A-4F66-B064-79B99647055C}">
   <dimension ref="B1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29843,7 +29909,7 @@
         <v>172</v>
       </c>
       <c r="C2" s="78" t="s">
-        <v>1190</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="19.5" thickBot="1">
@@ -29851,99 +29917,99 @@
         <v>583</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="18.75">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="109" t="s">
         <v>604</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>1192</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="108"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="82"/>
     </row>
     <row r="6" spans="2:3" ht="18.75">
-      <c r="B6" s="108"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="81" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="108"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="82"/>
     </row>
     <row r="8" spans="2:3" ht="18.75">
-      <c r="B8" s="108"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="81" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="18.75">
-      <c r="B9" s="108"/>
+      <c r="B9" s="110"/>
       <c r="C9" s="81" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="18.75">
-      <c r="B10" s="108"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="81" t="s">
-        <v>1196</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="18.75">
-      <c r="B11" s="108"/>
+      <c r="B11" s="110"/>
       <c r="C11" s="81" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="18.75">
-      <c r="B12" s="108"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="81" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="18.75">
-      <c r="B13" s="108"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="81" t="s">
-        <v>1199</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="18.75">
-      <c r="B14" s="108"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="81" t="s">
-        <v>1200</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="18.75">
-      <c r="B15" s="108"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="81" t="s">
-        <v>1201</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B16" s="109"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="80" t="s">
-        <v>1202</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="109" t="s">
         <v>306</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="108"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="82"/>
     </row>
     <row r="19" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B19" s="109"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="80" t="s">
         <v>1110</v>
       </c>
@@ -29953,7 +30019,7 @@
         <v>558</v>
       </c>
       <c r="C20" s="83" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="19.5" thickBot="1">
@@ -29961,25 +30027,25 @@
         <v>227</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="18.75">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="109" t="s">
         <v>348</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>1206</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="108"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="82"/>
     </row>
     <row r="24" spans="2:3" ht="38.25" thickBot="1">
-      <c r="B24" s="109"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="84" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="38.25" thickBot="1">
@@ -29987,25 +30053,25 @@
         <v>473</v>
       </c>
       <c r="C25" s="87" t="s">
-        <v>1208</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="18.75">
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="109" t="s">
         <v>505</v>
       </c>
       <c r="C26" s="88" t="s">
-        <v>1209</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="108"/>
+      <c r="B27" s="110"/>
       <c r="C27" s="82"/>
     </row>
     <row r="28" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B28" s="109"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="84" t="s">
-        <v>1210</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="19.5" thickBot="1">
@@ -30013,7 +30079,7 @@
         <v>278</v>
       </c>
       <c r="C29" s="89" t="s">
-        <v>1211</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="19.5" thickBot="1">
@@ -30021,7 +30087,7 @@
         <v>374</v>
       </c>
       <c r="C30" s="89" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="19.5" thickBot="1">
@@ -30029,15 +30095,15 @@
         <v>437</v>
       </c>
       <c r="C31" s="90" t="s">
-        <v>1213</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="18.75">
       <c r="B32" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="C32" s="113" t="s">
-        <v>1214</v>
+      <c r="C32" s="104" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="19.5" thickBot="1">
@@ -30045,25 +30111,25 @@
         <v>249</v>
       </c>
       <c r="C33" s="91" t="s">
-        <v>1215</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="18.75">
-      <c r="B34" s="107" t="s">
+      <c r="B34" s="109" t="s">
         <v>326</v>
       </c>
       <c r="C34" s="92" t="s">
-        <v>1216</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="108"/>
+      <c r="B35" s="110"/>
       <c r="C35" s="82"/>
     </row>
     <row r="36" spans="2:3" ht="38.25" thickBot="1">
-      <c r="B36" s="109"/>
+      <c r="B36" s="111"/>
       <c r="C36" s="91" t="s">
-        <v>1217</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="19.5" thickBot="1">
@@ -30071,61 +30137,61 @@
         <v>400</v>
       </c>
       <c r="C37" s="91" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="37.5">
-      <c r="B38" s="107" t="s">
+      <c r="B38" s="109" t="s">
         <v>535</v>
       </c>
       <c r="C38" s="92" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="39" spans="2:3">
-      <c r="B39" s="108"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="82"/>
     </row>
     <row r="40" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B40" s="109"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="91" t="s">
         <v>1129</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="18.75">
-      <c r="B41" s="107" t="s">
+      <c r="B41" s="109" t="s">
         <v>737</v>
       </c>
       <c r="C41" s="92" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="42" spans="2:3">
-      <c r="B42" s="108"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="82"/>
     </row>
     <row r="43" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B43" s="109"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="91" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="18.75">
-      <c r="B44" s="110" t="s">
+      <c r="B44" s="112" t="s">
         <v>986</v>
       </c>
       <c r="C44" s="93" t="s">
-        <v>1221</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="45" spans="2:3">
-      <c r="B45" s="111"/>
+      <c r="B45" s="113"/>
       <c r="C45" s="82"/>
     </row>
     <row r="46" spans="2:3" ht="38.25" thickBot="1">
-      <c r="B46" s="112"/>
+      <c r="B46" s="114"/>
       <c r="C46" s="94" t="s">
-        <v>1181</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="19.5" thickBot="1">
@@ -30133,25 +30199,25 @@
         <v>1001</v>
       </c>
       <c r="C47" s="94" t="s">
-        <v>1222</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="37.5">
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="109" t="s">
         <v>630</v>
       </c>
       <c r="C48" s="103" t="s">
-        <v>1223</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="49" spans="2:3">
-      <c r="B49" s="108"/>
+      <c r="B49" s="110"/>
       <c r="C49" s="82"/>
     </row>
     <row r="50" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B50" s="109"/>
+      <c r="B50" s="111"/>
       <c r="C50" s="80" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="19.5" thickBot="1">
@@ -30159,7 +30225,7 @@
         <v>656</v>
       </c>
       <c r="C51" s="80" t="s">
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="19.5" thickBot="1">
@@ -30167,35 +30233,35 @@
         <v>674</v>
       </c>
       <c r="C52" s="80" t="s">
-        <v>1225</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="18.75">
-      <c r="B53" s="107" t="s">
+      <c r="B53" s="109" t="s">
         <v>833</v>
       </c>
       <c r="C53" s="81" t="s">
-        <v>1226</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="108"/>
+      <c r="B54" s="110"/>
       <c r="C54" s="82"/>
     </row>
     <row r="55" spans="2:3" ht="37.5">
-      <c r="B55" s="108"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="81" t="s">
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="108"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="82"/>
     </row>
     <row r="57" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B57" s="109"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="80" t="s">
-        <v>1228</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="19.5" thickBot="1">
@@ -30203,7 +30269,7 @@
         <v>701</v>
       </c>
       <c r="C58" s="84" t="s">
-        <v>1229</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="19.5" thickBot="1">
@@ -30215,21 +30281,21 @@
       </c>
     </row>
     <row r="60" spans="2:3" ht="18.75">
-      <c r="B60" s="107" t="s">
+      <c r="B60" s="109" t="s">
         <v>766</v>
       </c>
       <c r="C60" s="81" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="61" spans="2:3">
-      <c r="B61" s="108"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="82"/>
     </row>
     <row r="62" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B62" s="109"/>
+      <c r="B62" s="111"/>
       <c r="C62" s="80" t="s">
-        <v>1154</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="38.25" thickBot="1">
@@ -30237,63 +30303,63 @@
         <v>793</v>
       </c>
       <c r="C63" s="80" t="s">
-        <v>1230</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="18.75">
-      <c r="B64" s="107" t="s">
+      <c r="B64" s="109" t="s">
         <v>816</v>
       </c>
       <c r="C64" s="81" t="s">
-        <v>1231</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="65" spans="2:3">
-      <c r="B65" s="108"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="82"/>
     </row>
     <row r="66" spans="2:3" ht="37.5">
-      <c r="B66" s="108"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="98" t="s">
-        <v>1232</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="67" spans="2:3">
-      <c r="B67" s="108"/>
+      <c r="B67" s="110"/>
       <c r="C67" s="82"/>
     </row>
     <row r="68" spans="2:3" ht="37.5">
-      <c r="B68" s="108"/>
+      <c r="B68" s="110"/>
       <c r="C68" s="81" t="s">
-        <v>1233</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="69" spans="2:3">
-      <c r="B69" s="108"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="82"/>
     </row>
     <row r="70" spans="2:3" ht="18.75">
-      <c r="B70" s="108"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="81" t="s">
-        <v>1234</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="71" spans="2:3">
-      <c r="B71" s="108"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="82"/>
     </row>
     <row r="72" spans="2:3" ht="38.25" thickBot="1">
-      <c r="B72" s="109"/>
+      <c r="B72" s="111"/>
       <c r="C72" s="80" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="57" thickBot="1">
       <c r="B73" s="79" t="s">
         <v>859</v>
       </c>
-      <c r="C73" s="84" t="s">
-        <v>1236</v>
+      <c r="C73" s="105" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="19.5" thickBot="1">
@@ -30301,7 +30367,7 @@
         <v>875</v>
       </c>
       <c r="C74" s="83" t="s">
-        <v>1237</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="38.25" thickBot="1">
@@ -30309,7 +30375,7 @@
         <v>894</v>
       </c>
       <c r="C75" s="80" t="s">
-        <v>1238</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="38.25" thickBot="1">
@@ -30317,7 +30383,7 @@
         <v>921</v>
       </c>
       <c r="C76" s="80" t="s">
-        <v>1239</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="19.5" thickBot="1">
@@ -30325,25 +30391,25 @@
         <v>950</v>
       </c>
       <c r="C77" s="99" t="s">
-        <v>1240</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="37.5">
-      <c r="B78" s="107" t="s">
+      <c r="B78" s="109" t="s">
         <v>970</v>
       </c>
       <c r="C78" s="100" t="s">
-        <v>1241</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="79" spans="2:3">
-      <c r="B79" s="108"/>
+      <c r="B79" s="110"/>
       <c r="C79" s="82"/>
     </row>
     <row r="80" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B80" s="109"/>
+      <c r="B80" s="111"/>
       <c r="C80" s="90" t="s">
-        <v>1242</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="19.5" thickBot="1">
@@ -30355,21 +30421,21 @@
       </c>
     </row>
     <row r="82" spans="2:3" ht="18.75">
-      <c r="B82" s="110" t="s">
+      <c r="B82" s="112" t="s">
         <v>1032</v>
       </c>
       <c r="C82" s="102" t="s">
-        <v>1243</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="83" spans="2:3">
-      <c r="B83" s="111"/>
+      <c r="B83" s="113"/>
       <c r="C83" s="82"/>
     </row>
     <row r="84" spans="2:3" ht="19.5" thickBot="1">
-      <c r="B84" s="112"/>
+      <c r="B84" s="114"/>
       <c r="C84" s="101" t="s">
-        <v>1183</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="19.5" thickBot="1">
@@ -30377,7 +30443,7 @@
         <v>1045</v>
       </c>
       <c r="C85" s="101" t="s">
-        <v>1244</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="19.5" thickBot="1">
@@ -30385,7 +30451,7 @@
         <v>1063</v>
       </c>
       <c r="C86" s="101" t="s">
-        <v>1245</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="19.5" thickBot="1">

</xml_diff>